<commit_message>
Add Cell Score Correlation Matrix analysis feature
Introduced callback_CellScoreCorrMatrix.m to enable correlation matrix analysis of cell scores from gene programs. Updated e_cellscorecorrmat to support Spearman correlation and additional outputs. Modified scgeatool.m for preference handling, and updated related assets and app files to support the new feature.
</commit_message>
<xml_diff>
--- a/assets/CellScores/cellscorecorrmat.xlsx
+++ b/assets/CellScores/cellscorecorrmat.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcai\Documents\GitHub\scGEAToolbox\assets\CellScores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\scGEAToolbox_prj\scGEAToolbox\assets\CellScores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96537303-716C-473B-B890-80CD9D09611E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61A9556-717A-493A-B970-241D83DD7DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3040" yWindow="3040" windowWidth="25800" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>ScoreType</t>
   </si>
@@ -60,12 +60,6 @@
     <t>IL7R,GPR183,KLRC1,GPR15,ARL4A,PTGER2,AUTS2,RARA,PIK3R1,LYAR,NUDT11,KLF3,CCND3,CLDND1,YPEL5</t>
   </si>
   <si>
-    <t>Li (2019) Mature macrophage</t>
-  </si>
-  <si>
-    <t>CD45,Adgre1,Lyz2</t>
-  </si>
-  <si>
     <t>Li (2019) M1 macrophage</t>
   </si>
   <si>
@@ -84,12 +78,6 @@
     <t>Igfbp4,Maf,Wwp1,Pcp4l1,Sepp1,C5ar1,Hpgds,Dpep2,Bmyc,Clec12a</t>
   </si>
   <si>
-    <t>Li (2019) Terminal maturation macrophage</t>
-  </si>
-  <si>
-    <t>Csf1r,Cebpb,Cd274,Itga4</t>
-  </si>
-  <si>
     <t>BEX3,STMN1,SOX4,LDHB,SKP1,SNRPE,ID3,SRP9,GSTP1,SRP14</t>
   </si>
   <si>
@@ -115,12 +103,6 @@
   </si>
   <si>
     <t>PEBP1,STAR,RARRES2, CLU,CYP21A2,CYP17A1,AKR1B1,NOV,TPD52L1,EPHX1</t>
-  </si>
-  <si>
-    <t>Han (2020) T_cell</t>
-  </si>
-  <si>
-    <t>CD3D,CD3E,CD3G,CD4,CD2,CD7,TRAC,TRBC1,LAT</t>
   </si>
   <si>
     <t>NDFIP2,MT1L,MYO1E,RRM2,CTLA4,AC022506.1,BHLHE40-AS1,TOX,AFAP1,PKMYT1,MAP1LC3A,MAMLD1,BATF3,RN7SL743P,TRAJ13,TNIP3,RNU6-786P,MIR3142HG,AC009088.2,HLA-DMA,MSC,AIMP2,ASB2,ADGRG1,AC023794.3,IGLV2-14,AC090152.1,TRBV27,TRAJ54,ENO1P1,NMB,LDHAP2,CCR5,MIR7848,AC145207.3,AL590133.2,RPL17-C18orf32,MIR155HG,ST8SIA1,FAM184A,AC078927.1,BUB1B,RAD51AP1,TIAM2,AKAP5,TRAJ22,AC008982.1,TRAJ42,EPOP,RNU6-1016P,C3orf14,CD200R1,TOX2,CCL4L2,FAM111B,IKZF4,RF02195,SETBP1,TRAJ32,RF00017,SNORD36A,AC115102.1,FCRL3,SLC5A2,INPP5F,AP005263.1,LINC01480,AL022067.1,NCS1,AC133644.2,AC120057.2,SLC27A2,CLECL1,BLOC1S5-TXNDC5,SECTM1,HIST1H2AJ,BCAT1,ENTPD1,RNY3P14,MIR4426,CCL3L1,AL928654.2,FAM3C2,RF00019,AL512625.3,AC006111.1,RNU6-645P,CDCA3,MT-TG,MT-TL2,RF00019,RAMP1,AL157871.4,SNORA61,TRGJP2,SNORA77,MELK,TNFRSF9,ADAM28,DTHD1,AC080023.2,SLC2A8,AL355816.1,LAIR2,AL354798.1,PTGES3P2,RDH10,SNORA70,RNU6-268P,AL360012.1,ST20-MTHFS,PDCD1,AC099329.1,AC009093.8,RN7SL653P,AC092069.1,RF02196,AC011247.2,CADM1,PDGFA,TRBV7-9,PIF1,RF00019,MSC-AS1,MT-TR,RF00019,RF00413,AL158071.2,CHN1,RN7SL559P,HAVCR2,KRT86,RN7SL246P,CCL3,RF00019,MS4A6A,RNY4P34,RNU7-1,AC009244.1,MRPS36P1,RAB38,CD86,TIGIT,CAMK1,ETV1,HECTD2,TRAJ6,TNFSF4,AC020978.5,AC090844.1,MIR6764,AC073261.1,SCARNA22,AC006064.4,LINC00271,TRAJ52,AC027319.1,KIR2DL4,RF00019,DRAIC,TRAJ4,VCAM1,AC009656.1,MYO7A,ATP8B4,CD200,LMCD1,AC013460.1,TIMD4,LINC01943,MIR4647,ZBTB20-AS1,RF02105,AC017002.3,AL035604.1,HMOX1,GNG4,AC145207.2,LINC00515,IL13,MT-TK,ZBED2,TMEM155,AL158071.3,TRAJ3,SNORD15B,RF00397,AC243829.4,SNORD104,GLDC,LINC02341,SNORD11,AC090498.1,HMGB1P17,PMCH,FNDC9,PPIAP45,MIR155,CXCL13</t>
@@ -617,19 +599,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="70.140625" customWidth="1"/>
-    <col min="2" max="2" width="48.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="70.1796875" customWidth="1"/>
+    <col min="2" max="2" width="48.54296875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -637,87 +619,87 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -725,7 +707,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -733,7 +715,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -741,31 +723,31 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="1" t="s">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="1" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>46</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -773,7 +755,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -781,47 +763,47 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="1" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -829,7 +811,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -837,7 +819,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -845,7 +827,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -853,7 +835,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -861,7 +843,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -869,7 +851,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -877,7 +859,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -885,7 +867,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -893,7 +875,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -901,7 +883,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -909,73 +891,49 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>69</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B37" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B38" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B39" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>76</v>
-      </c>
       <c r="B40" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>77</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
         <v>78</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>79</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A52" xr:uid="{16A74B7B-773D-4D2D-A1EA-E16BA506650B}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A49" xr:uid="{16A74B7B-773D-4D2D-A1EA-E16BA506650B}">
       <formula1>COUNTIF($A:$A,A1)&lt;2</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>